<commit_message>
Maven, Git, Jquery をwordで作成
</commit_message>
<xml_diff>
--- a/ノート.xlsx
+++ b/ノート.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keite\OneDrive\デスクトップ\ノート\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3762749D-282A-4B29-9B07-7A1B6D78DB63}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623F0FCD-5FA1-4D2A-95D7-A56F6002343B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8952" activeTab="5" xr2:uid="{23A547DA-F9B8-4989-9B8D-BFB06737F436}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8952" activeTab="2" xr2:uid="{23A547DA-F9B8-4989-9B8D-BFB06737F436}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel ショートカットキー" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="Maven" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">git!$A$1:$AC$176</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">jquery!$A$1:$AC$109</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Maven!$A$1:$AK$332</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="322">
   <si>
     <t>エクセル ショートカットキー</t>
   </si>
@@ -991,9 +993,6 @@
     <t>https://qiita.com/ASHITSUBO/items/6c2aa8dd55043781c6b4</t>
   </si>
   <si>
-    <t>Project Object Model (POM) という考え方に基づき、プロジェクトのビルド、テスト、ドキュメンテーション、成果物の配備など、プロジェクトのライフサイクル全体を管理</t>
-  </si>
-  <si>
     <t>ローカル環境にある全てのプロジェクトの間でライブラリを共有することがでる</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1636,6 +1635,13 @@
       <t>ハイジョ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Project Object Model (POM) という考え方に基づき、プロジェクトのビルド、テスト、ドキュメンテーション、成果物の配備など、</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロジェクトのライフサイクル全体を管理</t>
   </si>
 </sst>
 </file>
@@ -3273,8 +3279,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>166254</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3289,8 +3295,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="259080" y="10012680"/>
-          <a:ext cx="3642360" cy="472440"/>
+          <a:off x="264622" y="9741131"/>
+          <a:ext cx="3725487" cy="400396"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3341,15 +3347,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>83127</xdr:colOff>
+      <xdr:colOff>83128</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>23357</xdr:rowOff>
+      <xdr:rowOff>69273</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3372,8 +3378,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="326967" y="14279880"/>
-          <a:ext cx="8001693" cy="5738357"/>
+          <a:off x="326968" y="14523720"/>
+          <a:ext cx="6630092" cy="5784273"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6018,64 +6024,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>23578</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>122380</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F3179EE-BFB7-4336-9DEA-712E27CA5776}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="6926580"/>
-          <a:ext cx="8291278" cy="5311600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100" cap="sq">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6100,7 +6048,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6133,16 +6081,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>30</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>57</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>152975</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>130162</xdr:rowOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>99682</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6158,7 +6106,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -6171,7 +6119,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7414260" y="14211300"/>
+          <a:off x="342900" y="18067020"/>
           <a:ext cx="6637595" cy="7178662"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6199,13 +6147,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>168222</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>190715</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6222,7 +6170,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6257,13 +6205,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>198702</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>136</xdr:row>
       <xdr:rowOff>152587</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6280,7 +6228,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6315,13 +6263,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>221563</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>147</xdr:row>
       <xdr:rowOff>160209</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6338,7 +6286,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6372,130 +6320,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>198702</xdr:colOff>
-      <xdr:row>149</xdr:row>
-      <xdr:rowOff>206071</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="図 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9186F5F3-D98E-416F-AE00-F75D9EF75021}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="312420" y="37764720"/>
-          <a:ext cx="6713802" cy="3817951"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100" cap="sq">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>133</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>57</xdr:col>
-      <xdr:colOff>183460</xdr:colOff>
-      <xdr:row>149</xdr:row>
-      <xdr:rowOff>198452</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="図 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69637FF7-11A9-4CAD-A5C3-5B84DB745C11}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7383780" y="37749480"/>
-          <a:ext cx="6698560" cy="3825572"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="38100" cap="sq">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="43000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>68898</xdr:colOff>
-      <xdr:row>166</xdr:row>
+      <xdr:row>183</xdr:row>
       <xdr:rowOff>129767</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6512,7 +6344,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -6547,13 +6379,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>243</xdr:row>
+      <xdr:row>260</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>718</xdr:colOff>
-      <xdr:row>308</xdr:row>
+      <xdr:row>325</xdr:row>
       <xdr:rowOff>207044</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6562,6 +6394,198 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCD82CC8-6C9C-4A35-A353-2B00D26701BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="89626440"/>
+          <a:ext cx="8291278" cy="15050804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>83538</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>68249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="図 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDE48840-AFA1-4909-9DF7-B73AA7B3A9A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="327378" y="34358249"/>
+          <a:ext cx="3254022" cy="3817951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>60628</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>183149</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="図 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E7D5D2B-26D6-476D-B1A1-C101C763F298}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3901440" y="34350628"/>
+          <a:ext cx="3109229" cy="3825572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>122543</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>76642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="図 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22C3ADF3-8A30-4C3D-8DAF-F34C400647F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6583,8 +6607,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="89626440"/>
-          <a:ext cx="8291278" cy="15050804"/>
+          <a:off x="243840" y="6858000"/>
+          <a:ext cx="7193903" cy="5105842"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7062,10 +7086,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" s="27" t="s">
         <v>290</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
@@ -7085,8 +7109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDB2AB0-A546-4A8E-8971-A30FCE69DD5B}">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AC81" sqref="AC81"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.19921875" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -7305,10 +7329,13 @@
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="https://jquery.com/" xr:uid="{9DC5E483-AAA2-4A67-909C-733A8AADC052}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="61" orientation="portrait" r:id="rId2"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="49" max="28" man="1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="30" max="28" man="1"/>
+    <brk id="53" max="28" man="1"/>
+    <brk id="91" max="28" man="1"/>
   </rowBreaks>
   <drawing r:id="rId3"/>
 </worksheet>
@@ -7316,9 +7343,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE4776A-9D9A-4C8B-B437-61DD6B39244F}">
-  <dimension ref="A1:AB176"/>
+  <dimension ref="A1:Z176"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="P127" sqref="P127"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.19921875" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
@@ -7355,56 +7384,56 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:26" x14ac:dyDescent="0.45">
       <c r="B27" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.45">
-      <c r="T28" s="1" t="s">
+    <row r="28" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="R28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="U28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AB28" s="1" t="s">
+      <c r="Z28" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.45">
-      <c r="T29" s="5" t="s">
+    <row r="29" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="R29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="W29" s="1" t="s">
+      <c r="U29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AB29" s="1" t="s">
+      <c r="Z29" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.45">
-      <c r="T30" s="1" t="s">
+    <row r="30" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="R30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W30" s="1" t="s">
+      <c r="U30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AB30" s="1" t="s">
+      <c r="Z30" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.45">
-      <c r="T31" s="5" t="s">
+    <row r="31" spans="2:26" x14ac:dyDescent="0.45">
+      <c r="R31" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="W31" s="1" t="s">
+      <c r="U31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AB31" s="1" t="s">
+      <c r="Z31" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:26" x14ac:dyDescent="0.45">
       <c r="N32" s="5"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.45">
@@ -7931,12 +7960,15 @@
   <hyperlinks>
     <hyperlink ref="B85" r:id="rId1" xr:uid="{A82D48B7-7655-4A0E-BEAB-14D636BEF777}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="72" orientation="portrait" r:id="rId2"/>
-  <rowBreaks count="3" manualBreakCount="3">
-    <brk id="47" max="16383" man="1"/>
-    <brk id="95" max="16383" man="1"/>
-    <brk id="136" max="16383" man="1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId2"/>
+  <rowBreaks count="5" manualBreakCount="5">
+    <brk id="41" max="28" man="1"/>
+    <brk id="46" max="16383" man="1"/>
+    <brk id="88" max="28" man="1"/>
+    <brk id="128" max="28" man="1"/>
+    <brk id="155" max="28" man="1"/>
   </rowBreaks>
   <drawing r:id="rId3"/>
 </worksheet>
@@ -7955,62 +7987,62 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B3" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="H3" s="25" t="s">
         <v>284</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" s="25" t="s">
+        <v>285</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>286</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B6" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="H6" s="25" t="s">
         <v>311</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" s="25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" s="25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B10" s="25" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B12" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B13" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -8023,7 +8055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581CF4D2-83F5-436B-BC18-77312C6749D6}">
   <dimension ref="A1:Z306"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A289" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.19921875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
   <cols>
@@ -8032,202 +8064,202 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B3" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B4" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L4" s="25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B5" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B37" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="C37" s="25" t="s">
         <v>274</v>
-      </c>
-      <c r="C37" s="25" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C38" s="25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C39" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" s="25" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C65" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C73" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D73" s="25" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C92" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C188" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C189" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="215" spans="25:26" x14ac:dyDescent="0.45">
       <c r="Y215" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="Z215" s="25" t="s">
         <v>292</v>
-      </c>
-      <c r="Z215" s="25" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="222" spans="25:26" x14ac:dyDescent="0.45">
       <c r="Y222" s="25" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Z222" s="25" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="248" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C248" s="25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="264" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C264" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="271" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C271" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="272" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C272" s="25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="280" spans="24:24" x14ac:dyDescent="0.45">
       <c r="X280" s="31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="281" spans="24:24" x14ac:dyDescent="0.45">
       <c r="X281" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="283" spans="24:24" x14ac:dyDescent="0.45">
       <c r="X283" s="25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="284" spans="24:24" x14ac:dyDescent="0.45">
       <c r="X284" s="25" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="291" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C291" s="25" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="298" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C298" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D298" s="25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="299" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D299" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="301" spans="3:12" x14ac:dyDescent="0.45">
       <c r="C301" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D301" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="302" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D302" s="25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L302" s="25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="303" spans="3:12" x14ac:dyDescent="0.45">
       <c r="D303" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="L303" s="25" t="s">
         <v>307</v>
-      </c>
-      <c r="L303" s="25" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="305" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C305" s="25" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D305" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="306" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C306" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -8240,10 +8272,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD51629F-D2F9-40A8-90CA-2774CDC49A29}">
-  <dimension ref="A1:L315"/>
+  <dimension ref="A1:L332"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AK12" sqref="AK12"/>
+    <sheetView showGridLines="0" topLeftCell="A247" zoomScale="25" zoomScaleNormal="25" zoomScaleSheetLayoutView="10" workbookViewId="0">
+      <selection activeCell="AI334" sqref="AI334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.19921875" defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -8258,458 +8290,470 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B3" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="21" t="s">
-        <v>193</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B5" s="21" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B30" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B56" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B57" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B59" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B60" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B62" s="22" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B113" s="22" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B96" s="22" t="s">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B126" s="22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B127" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B150" s="22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B169" s="22" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B170" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="G170" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B172" s="22" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B109" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B110" s="21" t="s">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B186" s="22" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B187" s="21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B188" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B190" s="22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B191" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B193" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B194" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B195" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B197" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B198" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B199" s="21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B200" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C200" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B201" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C201" s="21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B202" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C202" s="21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B204" s="22" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B205" s="21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B206" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B207" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B208" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B209" s="21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B211" s="21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B212" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B213" s="21" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B214" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B216" s="22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B217" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B218" s="21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B220" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B221" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B222" s="23" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B223" s="21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B225" s="22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B226" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="C226" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B227" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="C227" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="228" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C228" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="D228" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B229" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C229" s="21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B231" s="24" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B232" s="21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B233" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B235" s="24" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B236" s="21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B237" s="21" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B239" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B240" s="21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="241" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B241" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="242" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B242" s="21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="243" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B243" s="21" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="245" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B245" s="22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="246" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B246" s="21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="248" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B248" s="22" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B133" s="22" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B152" s="22" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B153" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="G153" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B155" s="22" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B169" s="22" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B170" s="21" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B171" s="21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B173" s="22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B174" s="21" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B176" s="21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B177" s="21" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B178" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B180" s="21" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B181" s="21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B182" s="21" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B183" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C183" s="21" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B184" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C184" s="21" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B185" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C185" s="21" t="s">
+    <row r="249" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B249" s="21" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B187" s="22" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B188" s="21" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B189" s="21" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B190" s="21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B191" s="21" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B192" s="21" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B194" s="21" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B195" s="21" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B196" s="21" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B197" s="21" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B199" s="22" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B200" s="21" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B201" s="21" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B203" s="21" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B204" s="21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B205" s="23" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B206" s="21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B208" s="22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B209" s="21" t="s">
-        <v>245</v>
-      </c>
-      <c r="C209" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B210" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="C210" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C211" s="21" t="s">
-        <v>245</v>
-      </c>
-      <c r="D211" s="21" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B212" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="C212" s="21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B214" s="24" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B215" s="21" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B216" s="21" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B218" s="24" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B219" s="21" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B220" s="21" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B222" s="21" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B223" s="21" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="224" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B224" s="21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B225" s="21" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B226" s="21" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B228" s="22" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B229" s="21" t="s">
+      <c r="C249" s="21" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B231" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B232" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C232" s="21" t="s">
+    <row r="250" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B250" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C250" s="21" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B233" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="C233" s="21" t="s">
+    <row r="252" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B252" s="21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="253" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B253" s="21" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B235" s="21" t="s">
+    <row r="255" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B255" s="21" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B236" s="21" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B238" s="21" t="s">
+    <row r="256" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B256" s="21" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B239" s="21" t="s">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B258" s="22" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B241" s="22" t="s">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B259" s="21" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B242" s="21" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A311" s="21" t="s">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A328" s="21" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A312" s="21" t="s">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A329" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="L312" s="11" t="s">
+      <c r="L329" s="11" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A313" s="21" t="s">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A330" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="L313" s="11" t="s">
+      <c r="L330" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A314" s="21" t="s">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A331" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="L314" s="11" t="s">
+      <c r="L331" s="11" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A315" s="21" t="s">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A332" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="L315" s="11" t="s">
+      <c r="L332" s="11" t="s">
         <v>188</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="G153" r:id="rId1" xr:uid="{26E1A52C-E795-4717-B3BD-A9192B4D5E70}"/>
-    <hyperlink ref="L314" r:id="rId2" xr:uid="{F97ED89C-D901-4D9E-8FAE-8C8818EC41C3}"/>
-    <hyperlink ref="L313" r:id="rId3" xr:uid="{0003F45E-9974-40D4-AF05-95B62288A6F7}"/>
-    <hyperlink ref="L315" r:id="rId4" xr:uid="{93BDE159-FDC5-44C4-8BF1-F01BB5269328}"/>
-    <hyperlink ref="L312" r:id="rId5" xr:uid="{F60C4C2F-25B2-4A78-86AF-34EDA6C59A29}"/>
+    <hyperlink ref="G170" r:id="rId1" xr:uid="{26E1A52C-E795-4717-B3BD-A9192B4D5E70}"/>
+    <hyperlink ref="L331" r:id="rId2" xr:uid="{F97ED89C-D901-4D9E-8FAE-8C8818EC41C3}"/>
+    <hyperlink ref="L330" r:id="rId3" xr:uid="{0003F45E-9974-40D4-AF05-95B62288A6F7}"/>
+    <hyperlink ref="L332" r:id="rId4" xr:uid="{93BDE159-FDC5-44C4-8BF1-F01BB5269328}"/>
+    <hyperlink ref="L329" r:id="rId5" xr:uid="{F60C4C2F-25B2-4A78-86AF-34EDA6C59A29}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="42" orientation="portrait" r:id="rId6"/>
-  <rowBreaks count="4" manualBreakCount="4">
-    <brk id="60" max="16383" man="1"/>
-    <brk id="108" max="16383" man="1"/>
-    <brk id="153" max="16383" man="1"/>
-    <brk id="239" max="16383" man="1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="74" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId6"/>
+  <rowBreaks count="6" manualBreakCount="6">
+    <brk id="57" max="36" man="1"/>
+    <brk id="111" max="16383" man="1"/>
+    <brk id="170" max="36" man="1"/>
+    <brk id="189" max="36" man="1"/>
+    <brk id="246" max="16383" man="1"/>
+    <brk id="297" max="36" man="1"/>
   </rowBreaks>
+  <colBreaks count="2" manualBreakCount="2">
+    <brk id="37" max="1048575" man="1"/>
+    <brk id="40" min="58" max="124" man="1"/>
+  </colBreaks>
   <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>